<commit_message>
:sparkles: convert scheduler to void type, to avoid double read excel
</commit_message>
<xml_diff>
--- a/src/main/resources/SpeedSendCountryMapping.xlsx
+++ b/src/main/resources/SpeedSendCountryMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kerjaan\training\cimbexcel\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F40DF0E-2547-42F7-8421-4A9DE4485E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA975B2F-497D-4094-8B35-F2B442784B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Bank List" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Bank List'!$B$1:$G$406</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Bank List'!$B$1:$G$401</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2689" uniqueCount="842">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2659" uniqueCount="832">
   <si>
     <t>SWIFT_CODE</t>
   </si>
@@ -2524,36 +2524,6 @@
   </si>
   <si>
     <t>TAIPEI FUBON COMMERCIAL BANK CO., LTD.</t>
-  </si>
-  <si>
-    <t>109-130508-001053</t>
-  </si>
-  <si>
-    <t>TAISHIN INTERNATIONAL BANK CO.,LTD</t>
-  </si>
-  <si>
-    <t>109-130508-001054</t>
-  </si>
-  <si>
-    <t>TAIWAN BUSINESS BANK</t>
-  </si>
-  <si>
-    <t>109-130508-001055</t>
-  </si>
-  <si>
-    <t>TAIWAN COOPERATIVE BANK, LTD.</t>
-  </si>
-  <si>
-    <t>109-130508-001056</t>
-  </si>
-  <si>
-    <t>TAIWAN SHIN KONG COMMERCIAL BANK CO., LTD</t>
-  </si>
-  <si>
-    <t>109-130508-001057</t>
-  </si>
-  <si>
-    <t>TORONTO-DOMINION BANK</t>
   </si>
 </sst>
 </file>
@@ -2842,10 +2812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z990"/>
+  <dimension ref="A1:Z985"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A401" workbookViewId="0">
-      <selection activeCell="C411" sqref="C411"/>
+      <selection activeCell="D413" sqref="D413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19404,25 +19374,13 @@
       <c r="Z401" s="3"/>
     </row>
     <row r="402" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A402" s="4" t="s">
-        <v>832</v>
-      </c>
-      <c r="B402" s="4" t="s">
-        <v>832</v>
-      </c>
-      <c r="C402" s="4" t="s">
-        <v>833</v>
-      </c>
-      <c r="D402" s="4" t="s">
-        <v>558</v>
-      </c>
-      <c r="E402" s="4"/>
-      <c r="F402" s="4" t="s">
-        <v>559</v>
-      </c>
-      <c r="G402" s="4" t="s">
-        <v>560</v>
-      </c>
+      <c r="A402" s="3"/>
+      <c r="B402" s="3"/>
+      <c r="C402" s="3"/>
+      <c r="D402" s="3"/>
+      <c r="E402" s="3"/>
+      <c r="F402" s="3"/>
+      <c r="G402" s="3"/>
       <c r="H402" s="3"/>
       <c r="I402" s="3"/>
       <c r="J402" s="3"/>
@@ -19444,25 +19402,13 @@
       <c r="Z402" s="3"/>
     </row>
     <row r="403" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A403" s="4" t="s">
-        <v>834</v>
-      </c>
-      <c r="B403" s="4" t="s">
-        <v>834</v>
-      </c>
-      <c r="C403" s="4" t="s">
-        <v>835</v>
-      </c>
-      <c r="D403" s="4" t="s">
-        <v>558</v>
-      </c>
-      <c r="E403" s="4"/>
-      <c r="F403" s="4" t="s">
-        <v>559</v>
-      </c>
-      <c r="G403" s="4" t="s">
-        <v>560</v>
-      </c>
+      <c r="A403" s="3"/>
+      <c r="B403" s="3"/>
+      <c r="C403" s="3"/>
+      <c r="D403" s="3"/>
+      <c r="E403" s="3"/>
+      <c r="F403" s="3"/>
+      <c r="G403" s="3"/>
       <c r="H403" s="3"/>
       <c r="I403" s="3"/>
       <c r="J403" s="3"/>
@@ -19484,25 +19430,13 @@
       <c r="Z403" s="3"/>
     </row>
     <row r="404" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A404" s="4" t="s">
-        <v>836</v>
-      </c>
-      <c r="B404" s="4" t="s">
-        <v>836</v>
-      </c>
-      <c r="C404" s="4" t="s">
-        <v>837</v>
-      </c>
-      <c r="D404" s="4" t="s">
-        <v>558</v>
-      </c>
-      <c r="E404" s="4"/>
-      <c r="F404" s="4" t="s">
-        <v>559</v>
-      </c>
-      <c r="G404" s="4" t="s">
-        <v>560</v>
-      </c>
+      <c r="A404" s="3"/>
+      <c r="B404" s="3"/>
+      <c r="C404" s="3"/>
+      <c r="D404" s="3"/>
+      <c r="E404" s="3"/>
+      <c r="F404" s="3"/>
+      <c r="G404" s="3"/>
       <c r="H404" s="3"/>
       <c r="I404" s="3"/>
       <c r="J404" s="3"/>
@@ -19524,25 +19458,13 @@
       <c r="Z404" s="3"/>
     </row>
     <row r="405" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A405" s="4" t="s">
-        <v>838</v>
-      </c>
-      <c r="B405" s="4" t="s">
-        <v>838</v>
-      </c>
-      <c r="C405" s="4" t="s">
-        <v>839</v>
-      </c>
-      <c r="D405" s="4" t="s">
-        <v>558</v>
-      </c>
-      <c r="E405" s="4"/>
-      <c r="F405" s="4" t="s">
-        <v>559</v>
-      </c>
-      <c r="G405" s="4" t="s">
-        <v>560</v>
-      </c>
+      <c r="A405" s="3"/>
+      <c r="B405" s="3"/>
+      <c r="C405" s="3"/>
+      <c r="D405" s="3"/>
+      <c r="E405" s="3"/>
+      <c r="F405" s="3"/>
+      <c r="G405" s="3"/>
       <c r="H405" s="3"/>
       <c r="I405" s="3"/>
       <c r="J405" s="3"/>
@@ -19564,25 +19486,13 @@
       <c r="Z405" s="3"/>
     </row>
     <row r="406" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A406" s="4" t="s">
-        <v>840</v>
-      </c>
-      <c r="B406" s="4" t="s">
-        <v>840</v>
-      </c>
-      <c r="C406" s="4" t="s">
-        <v>841</v>
-      </c>
-      <c r="D406" s="4" t="s">
-        <v>558</v>
-      </c>
-      <c r="E406" s="4"/>
-      <c r="F406" s="4" t="s">
-        <v>559</v>
-      </c>
-      <c r="G406" s="4" t="s">
-        <v>560</v>
-      </c>
+      <c r="A406" s="3"/>
+      <c r="B406" s="3"/>
+      <c r="C406" s="3"/>
+      <c r="D406" s="3"/>
+      <c r="E406" s="3"/>
+      <c r="F406" s="3"/>
+      <c r="G406" s="3"/>
       <c r="H406" s="3"/>
       <c r="I406" s="3"/>
       <c r="J406" s="3"/>
@@ -35815,148 +35725,8 @@
       <c r="Y985" s="3"/>
       <c r="Z985" s="3"/>
     </row>
-    <row r="986" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A986" s="3"/>
-      <c r="B986" s="3"/>
-      <c r="C986" s="3"/>
-      <c r="D986" s="3"/>
-      <c r="E986" s="3"/>
-      <c r="F986" s="3"/>
-      <c r="G986" s="3"/>
-      <c r="H986" s="3"/>
-      <c r="I986" s="3"/>
-      <c r="J986" s="3"/>
-      <c r="K986" s="3"/>
-      <c r="L986" s="3"/>
-      <c r="M986" s="3"/>
-      <c r="N986" s="3"/>
-      <c r="O986" s="3"/>
-      <c r="P986" s="3"/>
-      <c r="Q986" s="3"/>
-      <c r="R986" s="3"/>
-      <c r="S986" s="3"/>
-      <c r="T986" s="3"/>
-      <c r="U986" s="3"/>
-      <c r="V986" s="3"/>
-      <c r="W986" s="3"/>
-      <c r="X986" s="3"/>
-      <c r="Y986" s="3"/>
-      <c r="Z986" s="3"/>
-    </row>
-    <row r="987" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A987" s="3"/>
-      <c r="B987" s="3"/>
-      <c r="C987" s="3"/>
-      <c r="D987" s="3"/>
-      <c r="E987" s="3"/>
-      <c r="F987" s="3"/>
-      <c r="G987" s="3"/>
-      <c r="H987" s="3"/>
-      <c r="I987" s="3"/>
-      <c r="J987" s="3"/>
-      <c r="K987" s="3"/>
-      <c r="L987" s="3"/>
-      <c r="M987" s="3"/>
-      <c r="N987" s="3"/>
-      <c r="O987" s="3"/>
-      <c r="P987" s="3"/>
-      <c r="Q987" s="3"/>
-      <c r="R987" s="3"/>
-      <c r="S987" s="3"/>
-      <c r="T987" s="3"/>
-      <c r="U987" s="3"/>
-      <c r="V987" s="3"/>
-      <c r="W987" s="3"/>
-      <c r="X987" s="3"/>
-      <c r="Y987" s="3"/>
-      <c r="Z987" s="3"/>
-    </row>
-    <row r="988" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A988" s="3"/>
-      <c r="B988" s="3"/>
-      <c r="C988" s="3"/>
-      <c r="D988" s="3"/>
-      <c r="E988" s="3"/>
-      <c r="F988" s="3"/>
-      <c r="G988" s="3"/>
-      <c r="H988" s="3"/>
-      <c r="I988" s="3"/>
-      <c r="J988" s="3"/>
-      <c r="K988" s="3"/>
-      <c r="L988" s="3"/>
-      <c r="M988" s="3"/>
-      <c r="N988" s="3"/>
-      <c r="O988" s="3"/>
-      <c r="P988" s="3"/>
-      <c r="Q988" s="3"/>
-      <c r="R988" s="3"/>
-      <c r="S988" s="3"/>
-      <c r="T988" s="3"/>
-      <c r="U988" s="3"/>
-      <c r="V988" s="3"/>
-      <c r="W988" s="3"/>
-      <c r="X988" s="3"/>
-      <c r="Y988" s="3"/>
-      <c r="Z988" s="3"/>
-    </row>
-    <row r="989" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A989" s="3"/>
-      <c r="B989" s="3"/>
-      <c r="C989" s="3"/>
-      <c r="D989" s="3"/>
-      <c r="E989" s="3"/>
-      <c r="F989" s="3"/>
-      <c r="G989" s="3"/>
-      <c r="H989" s="3"/>
-      <c r="I989" s="3"/>
-      <c r="J989" s="3"/>
-      <c r="K989" s="3"/>
-      <c r="L989" s="3"/>
-      <c r="M989" s="3"/>
-      <c r="N989" s="3"/>
-      <c r="O989" s="3"/>
-      <c r="P989" s="3"/>
-      <c r="Q989" s="3"/>
-      <c r="R989" s="3"/>
-      <c r="S989" s="3"/>
-      <c r="T989" s="3"/>
-      <c r="U989" s="3"/>
-      <c r="V989" s="3"/>
-      <c r="W989" s="3"/>
-      <c r="X989" s="3"/>
-      <c r="Y989" s="3"/>
-      <c r="Z989" s="3"/>
-    </row>
-    <row r="990" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A990" s="3"/>
-      <c r="B990" s="3"/>
-      <c r="C990" s="3"/>
-      <c r="D990" s="3"/>
-      <c r="E990" s="3"/>
-      <c r="F990" s="3"/>
-      <c r="G990" s="3"/>
-      <c r="H990" s="3"/>
-      <c r="I990" s="3"/>
-      <c r="J990" s="3"/>
-      <c r="K990" s="3"/>
-      <c r="L990" s="3"/>
-      <c r="M990" s="3"/>
-      <c r="N990" s="3"/>
-      <c r="O990" s="3"/>
-      <c r="P990" s="3"/>
-      <c r="Q990" s="3"/>
-      <c r="R990" s="3"/>
-      <c r="S990" s="3"/>
-      <c r="T990" s="3"/>
-      <c r="U990" s="3"/>
-      <c r="V990" s="3"/>
-      <c r="W990" s="3"/>
-      <c r="X990" s="3"/>
-      <c r="Y990" s="3"/>
-      <c r="Z990" s="3"/>
-    </row>
   </sheetData>
-  <autoFilter ref="B1:G406" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:G401" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>